<commit_message>
New Transport Buffer implementation
Added notification
Updated Development excel
</commit_message>
<xml_diff>
--- a/Development.xlsx
+++ b/Development.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\ISEC\SO2\Pratica\Trabalho\SOTaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D08916-3FA7-4F1A-83E0-90AE4F1334F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D6722A-E0A2-479B-ABF3-83651AEDC7F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11055" yWindow="825" windowWidth="21510" windowHeight="11430" firstSheet="1" activeTab="3" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
+    <workbookView xWindow="3030" yWindow="540" windowWidth="21510" windowHeight="11430" activeTab="1" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
   </bookViews>
   <sheets>
     <sheet name="CenDLL" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="81">
   <si>
     <t>Functionality</t>
   </si>
@@ -256,6 +256,33 @@
   </si>
   <si>
     <t>Print CMD messages about what is happening</t>
+  </si>
+  <si>
+    <t>Hold generic defines</t>
+  </si>
+  <si>
+    <t>Hold generic enums</t>
+  </si>
+  <si>
+    <t>Hold generic structs</t>
+  </si>
+  <si>
+    <t>Provide generic functionality</t>
+  </si>
+  <si>
+    <t>Printing format</t>
+  </si>
+  <si>
+    <t>Clean stdin</t>
+  </si>
+  <si>
+    <t>Check if string is empty</t>
+  </si>
+  <si>
+    <t>Check if string is a number</t>
+  </si>
+  <si>
+    <t>Clean String</t>
   </si>
 </sst>
 </file>
@@ -439,21 +466,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -492,40 +510,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableHeader" xfId="1" xr:uid="{14BB81CB-250E-410C-BBDF-11D0D22B1B10}"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
         </patternFill>
       </fill>
     </dxf>
@@ -539,7 +584,21 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -553,6 +612,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -560,21 +626,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -900,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B86DE73-C9EA-4FED-97AB-CCAFAE0E0C8C}">
-  <dimension ref="B2:E7"/>
+  <dimension ref="B2:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:XFD1048576"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,28 +978,137 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="3" t="s">
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E4" s="4"/>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E5" s="4"/>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="23"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="5"/>
+      <c r="B6" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="15"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="15"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="15"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="15"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="15"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="15"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="15"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E3:E6"/>
   </mergeCells>
+  <conditionalFormatting sqref="C3:C18">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
+      <formula>LEN(TRIM(C3))=0</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{582C28A6-C8BE-4D1F-9733-995A371E59B7}">
+            <xm:f>NOT(ISERROR(SEARCH("-",C3)))</xm:f>
+            <xm:f>"-"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C3:C18</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -955,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{958854CD-AF03-4FB5-B1A5-A2453B181DC1}">
   <dimension ref="B2:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,129 +1140,129 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="22" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="4"/>
+      <c r="C4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="5"/>
+      <c r="C5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="24"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="7"/>
+      <c r="C7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="E8" s="6"/>
+      <c r="C8" s="15"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="E9" s="6"/>
+      <c r="C9" s="15"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="18"/>
+      <c r="C10" s="15"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="18"/>
+      <c r="C11" s="15"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="18"/>
+      <c r="C12" s="15"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="15"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="15"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="18"/>
+      <c r="C15" s="15"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="18"/>
+      <c r="C16" s="15"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="18"/>
+      <c r="C17" s="15"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="18"/>
+      <c r="C18" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E3:E5"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C18">
-    <cfRule type="containsBlanks" dxfId="8" priority="1">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1133,8 +1294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829518F3-E732-4739-88CC-0EF1DA64B468}">
   <dimension ref="B2:E37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,260 +1318,270 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="C3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="E4" s="5"/>
+      <c r="C4" s="15"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="E5" s="22"/>
+      <c r="C5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="17"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="22"/>
+      <c r="E6" s="17"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="E7" s="22"/>
+      <c r="C7" s="15"/>
+      <c r="E7" s="17"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="E8" s="22"/>
+      <c r="C8" s="15"/>
+      <c r="E8" s="17"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="22"/>
+      <c r="E9" s="17"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="E10" s="8"/>
+      <c r="C10" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="E11" s="8"/>
+      <c r="C11" s="15"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="8"/>
+      <c r="C12" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="E13" s="8"/>
+      <c r="C13" s="15"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="8"/>
+      <c r="C14" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="E15" s="8"/>
+      <c r="C15" s="15"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="E16" s="8"/>
+      <c r="C16" s="15"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="E17" s="8"/>
+      <c r="C17" s="15"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="6"/>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="E19" s="6"/>
+      <c r="C19" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="18"/>
-      <c r="E20" s="6"/>
+      <c r="C20" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="18"/>
+      <c r="C21" s="15"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="18"/>
+      <c r="C22" s="15"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="18"/>
+      <c r="C24" s="15" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="18"/>
+      <c r="C25" s="15"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C26" s="18"/>
+      <c r="C26" s="15"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="18"/>
+      <c r="C28" s="15"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="18"/>
+      <c r="C29" s="15"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="18"/>
+      <c r="C30" s="15"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="18"/>
+      <c r="C31" s="15"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="18"/>
+      <c r="C32" s="15"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="18"/>
+      <c r="C33" s="15"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="18"/>
+      <c r="C34" s="15"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="18"/>
+      <c r="C35" s="15"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="18"/>
+      <c r="C36" s="15"/>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="19"/>
+      <c r="C37" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E3:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C37">
-    <cfRule type="containsBlanks" dxfId="5" priority="1">
+    <cfRule type="containsBlanks" dxfId="11" priority="1">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1442,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0EDB92-DEAA-412F-9746-22ECF9A3453C}">
   <dimension ref="B2:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,167 +1637,167 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="20" t="s">
+      <c r="C3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="21"/>
+      <c r="C4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="18"/>
+      <c r="C5" s="15"/>
       <c r="E5" s="27"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="22"/>
+      <c r="E6" s="17"/>
     </row>
     <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="22"/>
+      <c r="C7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="17"/>
     </row>
     <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="22"/>
+      <c r="C8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="17"/>
     </row>
     <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="22"/>
+      <c r="C10" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="17"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="18"/>
-      <c r="E11" s="22"/>
+      <c r="C11" s="15"/>
+      <c r="E11" s="17"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="E12" s="22"/>
+      <c r="C12" s="15"/>
+      <c r="E12" s="17"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="E13" s="22"/>
+      <c r="C13" s="15"/>
+      <c r="E13" s="17"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="E14" s="22"/>
+      <c r="C14" s="15"/>
+      <c r="E14" s="17"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="E15" s="8"/>
+      <c r="C15" s="15"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="E16" s="8"/>
+      <c r="C16" s="15"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="E17" s="8"/>
+      <c r="C17" s="15"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="E18" s="8"/>
+      <c r="C18" s="15"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="E19" s="8"/>
+      <c r="C19" s="15"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="8"/>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="8"/>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="8"/>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="6"/>
+      <c r="C23" s="3"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="6"/>
+      <c r="C24" s="3"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="6"/>
+      <c r="C25" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E3:E5"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C19">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+    <cfRule type="containsBlanks" dxfId="8" priority="1">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1682,16 +1853,16 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="3"/>
+      <c r="E3" s="22"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E4" s="4"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E5" s="4"/>
+      <c r="E5" s="23"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="5"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>
@@ -1732,16 +1903,16 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="3"/>
+      <c r="E3" s="22"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E4" s="4"/>
+      <c r="E4" s="23"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E5" s="4"/>
+      <c r="E5" s="23"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="5"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>

</xml_diff>

<commit_message>
ConTaxi Commands & CenTaxi choose taxi
</commit_message>
<xml_diff>
--- a/Development.xlsx
+++ b/Development.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\ISEC\SO2\Pratica\Trabalho\SOTaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D1124C-218A-4940-9D7B-F1A2505B8FAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AD3AFA-78CE-4BA7-930C-F897C15D6588}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="540" windowWidth="21510" windowHeight="11430" activeTab="1" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
   </bookViews>
   <sheets>
     <sheet name="CenDLL" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="84">
   <si>
     <t>Functionality</t>
   </si>
@@ -183,9 +183,6 @@
     <t>Autonomous movement</t>
   </si>
   <si>
-    <t>Autonomous transport interest requests</t>
-  </si>
-  <si>
     <t>Movement</t>
   </si>
   <si>
@@ -225,9 +222,6 @@
     <t>Send transport interest</t>
   </si>
   <si>
-    <t>Send transport interest (if automatic is off)</t>
-  </si>
-  <si>
     <t>Shutdown application</t>
   </si>
   <si>
@@ -292,6 +286,12 @@
   </si>
   <si>
     <t>Receive notification (from central) to leave</t>
+  </si>
+  <si>
+    <t>Named pipe</t>
+  </si>
+  <si>
+    <t>Named Pipe</t>
   </si>
 </sst>
 </file>
@@ -988,7 +988,7 @@
     </row>
     <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>6</v>
@@ -999,7 +999,7 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>6</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>6</v>
@@ -1017,7 +1017,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>10</v>
@@ -1026,7 +1026,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>6</v>
@@ -1035,7 +1035,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>6</v>
@@ -1043,7 +1043,7 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>6</v>
@@ -1051,7 +1051,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>6</v>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>6</v>
@@ -1104,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{958854CD-AF03-4FB5-B1A5-A2453B181DC1}">
-  <dimension ref="B2:E19"/>
+  <dimension ref="B2:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>6</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>6</v>
@@ -1160,7 +1160,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>10</v>
@@ -1169,7 +1169,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>6</v>
@@ -1178,21 +1178,24 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C8" s="15"/>
+      <c r="D8" t="s">
+        <v>82</v>
+      </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C9" s="15"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>6</v>
@@ -1201,13 +1204,15 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="15"/>
+        <v>47</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="15"/>
     </row>
@@ -1215,49 +1220,21 @@
       <c r="B13" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="15"/>
+      <c r="C13" s="15" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="15"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="15"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="15"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="15"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="15"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="15"/>
+      <c r="B14" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E3:E5"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C19">
+  <conditionalFormatting sqref="C3:C14">
     <cfRule type="containsBlanks" dxfId="8" priority="1">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
@@ -1281,7 +1258,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C3:C19</xm:sqref>
+          <xm:sqref>C3:C14</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1293,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829518F3-E732-4739-88CC-0EF1DA64B468}">
   <dimension ref="B2:E37"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,7 +1313,7 @@
     </row>
     <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>6</v>
@@ -1470,7 +1447,7 @@
       </c>
       <c r="C21" s="15"/>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
@@ -1479,7 +1456,7 @@
       </c>
       <c r="C22" s="15"/>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -1504,7 +1481,7 @@
       </c>
       <c r="C25" s="15"/>
       <c r="D25" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -1513,7 +1490,7 @@
       </c>
       <c r="C26" s="15"/>
       <c r="D26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
@@ -1528,7 +1505,9 @@
       <c r="B28" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="15"/>
+      <c r="C28" s="15" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
@@ -1536,7 +1515,7 @@
       </c>
       <c r="C29" s="15"/>
       <c r="D29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
@@ -1593,7 +1572,7 @@
       </c>
       <c r="C37" s="16"/>
       <c r="D37" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1634,10 +1613,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0EDB92-DEAA-412F-9746-22ECF9A3453C}">
-  <dimension ref="B2:E25"/>
+  <dimension ref="B2:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,7 +1651,7 @@
     </row>
     <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>6</v>
@@ -1681,9 +1660,11 @@
     </row>
     <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="15"/>
+        <v>52</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="E5" s="29"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1706,7 +1687,7 @@
     </row>
     <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>6</v>
@@ -1715,7 +1696,7 @@
     </row>
     <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>10</v>
@@ -1724,7 +1705,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>6</v>
@@ -1733,16 +1714,21 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C11" s="15"/>
+      <c r="D11" t="s">
+        <v>83</v>
+      </c>
       <c r="E11" s="17"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="15" t="s">
+        <v>10</v>
+      </c>
       <c r="E12" s="17"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -1754,69 +1740,89 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="E14" s="17"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="15" t="s">
+        <v>10</v>
+      </c>
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="15"/>
+      <c r="C16" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="9" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="15"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="9" t="s">
-        <v>50</v>
+      <c r="B18" s="18" t="s">
+        <v>61</v>
       </c>
       <c r="C18" s="15"/>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="15"/>
-      <c r="E19" s="5"/>
+      <c r="B19" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="5"/>
+      <c r="B20" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="15"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="5"/>
+      <c r="B21" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="5"/>
+      <c r="B22" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="3"/>
+      <c r="B23" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E3:E5"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C19">
+  <conditionalFormatting sqref="C3:C23">
     <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
@@ -1825,6 +1831,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -1840,7 +1847,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C3:C19</xm:sqref>
+          <xm:sqref>C3:C23</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
CenTaxi Commands & CenTaxi Settings
</commit_message>
<xml_diff>
--- a/Development.xlsx
+++ b/Development.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\ISEC\SO2\Pratica\Trabalho\SOTaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AD3AFA-78CE-4BA7-930C-F897C15D6588}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED989F4-AAD8-4492-9B00-3F8CD1673665}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
   </bookViews>
   <sheets>
     <sheet name="CenDLL" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="85">
   <si>
     <t>Functionality</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>Named Pipe</t>
+  </si>
+  <si>
+    <t>Needs to be looked</t>
   </si>
 </sst>
 </file>
@@ -1107,7 +1110,7 @@
   <dimension ref="B2:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829518F3-E732-4739-88CC-0EF1DA64B468}">
   <dimension ref="B2:E37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,7 +1407,9 @@
       <c r="B16" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="15"/>
+      <c r="C16" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -1547,24 +1552,33 @@
         <v>29</v>
       </c>
       <c r="C33" s="15"/>
+      <c r="D33" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="15"/>
+      <c r="C34" s="15" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="15"/>
+      <c r="C35" s="15" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="15"/>
+      <c r="C36" s="15" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="13" t="s">
@@ -1615,7 +1629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0EDB92-DEAA-412F-9746-22ECF9A3453C}">
   <dimension ref="B2:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -1909,8 +1923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{479F52BC-D323-484C-B995-079999EECDCA}">
   <dimension ref="B2:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
CenTaxi Map update + ConTaxi Map request
</commit_message>
<xml_diff>
--- a/Development.xlsx
+++ b/Development.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\ISEC\SO2\Pratica\Trabalho\SOTaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E04D53-71A0-41DC-9622-0128BE8BC6F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033A7022-3678-4770-B9B5-734891C739C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="1725" windowWidth="21510" windowHeight="11430" activeTab="2" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
+    <workbookView xWindow="3060" yWindow="1725" windowWidth="21510" windowHeight="11430" activeTab="3" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
   </bookViews>
   <sheets>
     <sheet name="CenDLL" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="89">
   <si>
     <t>Functionality</t>
   </si>
@@ -298,6 +298,15 @@
   </si>
   <si>
     <t>? Is it</t>
+  </si>
+  <si>
+    <t>Missing MapInfo</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Receive map</t>
   </si>
 </sst>
 </file>
@@ -481,7 +490,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1">
       <alignment horizontal="center" vertical="center"/>
@@ -561,6 +570,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1110,10 +1122,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{958854CD-AF03-4FB5-B1A5-A2453B181DC1}">
-  <dimension ref="B2:E14"/>
+  <dimension ref="B2:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,85 +1174,94 @@
       <c r="C5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="26"/>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="26"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C7" s="15" t="s">
         <v>10</v>
-      </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>6</v>
       </c>
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" t="s">
+      <c r="C9" s="15"/>
+      <c r="D9" t="s">
         <v>82</v>
       </c>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="15"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
+      <c r="C11" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C12" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="18" t="s">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="15"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
+      <c r="C13" s="15"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C14" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="20" t="s">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C15" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="E3:E6"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C14">
+  <conditionalFormatting sqref="C3:C15">
     <cfRule type="containsBlanks" dxfId="8" priority="1">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
@@ -1264,7 +1285,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C3:C14</xm:sqref>
+          <xm:sqref>C3:C15</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1276,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829518F3-E732-4739-88CC-0EF1DA64B468}">
   <dimension ref="B2:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1285,6 +1306,7 @@
     <col min="1" max="1" width="3.140625" customWidth="1"/>
     <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="48" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1314,7 +1336,12 @@
       <c r="B4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="15"/>
+      <c r="C4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>86</v>
+      </c>
       <c r="E4" s="26"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1348,7 +1375,12 @@
       <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
       <c r="E8" s="17"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -1634,8 +1666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0EDB92-DEAA-412F-9746-22ECF9A3453C}">
   <dimension ref="B2:E24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
TossRequests (Core | Taxi Position and Taxi State)
</commit_message>
<xml_diff>
--- a/Development.xlsx
+++ b/Development.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\ISEC\SO2\Pratica\Trabalho\SOTaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033A7022-3678-4770-B9B5-734891C739C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4058332A-65AC-4A8C-8980-840494E74335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="1725" windowWidth="21510" windowHeight="11430" activeTab="3" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21510" windowHeight="11430" activeTab="3" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
   </bookViews>
   <sheets>
     <sheet name="CenDLL" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="91">
   <si>
     <t>Functionality</t>
   </si>
@@ -195,9 +195,6 @@
     <t>Send new position (when enter new cell)</t>
   </si>
   <si>
-    <t>Autonomous show interest if between CDN</t>
-  </si>
-  <si>
     <t>Default CDN</t>
   </si>
   <si>
@@ -207,9 +204,6 @@
     <t>Receive notification (from central) about new transport</t>
   </si>
   <si>
-    <t>Movement (UP, DOWN, LEFT, RIGHT)</t>
-  </si>
-  <si>
     <t>Speed Up/Down (0.5)</t>
   </si>
   <si>
@@ -297,9 +291,6 @@
     <t>Needs to be looked</t>
   </si>
   <si>
-    <t>? Is it</t>
-  </si>
-  <si>
     <t>Missing MapInfo</t>
   </si>
   <si>
@@ -307,6 +298,21 @@
   </si>
   <si>
     <t>Receive map</t>
+  </si>
+  <si>
+    <t>Still need Step</t>
+  </si>
+  <si>
+    <t>Send new state</t>
+  </si>
+  <si>
+    <t>Missing Step</t>
+  </si>
+  <si>
+    <t>Event?</t>
+  </si>
+  <si>
+    <t>Autonomous interest if between CDN</t>
   </si>
 </sst>
 </file>
@@ -553,6 +559,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -570,16 +579,34 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableHeader" xfId="1" xr:uid="{14BB81CB-250E-410C-BBDF-11D0D22B1B10}"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1006,45 +1033,45 @@
     </row>
     <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="25" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="26"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>6</v>
@@ -1053,7 +1080,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>6</v>
@@ -1061,7 +1088,7 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>6</v>
@@ -1069,7 +1096,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>6</v>
@@ -1077,7 +1104,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>6</v>
@@ -1088,10 +1115,10 @@
     <mergeCell ref="E3:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C11">
-    <cfRule type="containsBlanks" dxfId="11" priority="1">
+    <cfRule type="containsBlanks" dxfId="14" priority="1">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1122,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{958854CD-AF03-4FB5-B1A5-A2453B181DC1}">
-  <dimension ref="B2:E15"/>
+  <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,40 +1181,40 @@
       <c r="C3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="25" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="26"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>10</v>
@@ -1196,7 +1223,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>6</v>
@@ -1205,24 +1232,27 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C10" s="15"/>
+      <c r="D10" t="s">
+        <v>89</v>
+      </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C11" s="15" t="s">
         <v>6</v>
@@ -1241,32 +1271,56 @@
       <c r="B13" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="15"/>
+      <c r="C13" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C15" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="16"/>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E3:E6"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C15">
-    <cfRule type="containsBlanks" dxfId="8" priority="1">
+  <conditionalFormatting sqref="C3:C12 C14:C16">
+    <cfRule type="containsBlanks" dxfId="11" priority="4">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="containsBlanks" dxfId="8" priority="1">
+      <formula>LEN(TRIM(C13))=0</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",C3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Yes",C13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1274,7 +1328,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{BB54431B-B164-4E14-BF24-00DF4041EFBE}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{BB54431B-B164-4E14-BF24-00DF4041EFBE}">
             <xm:f>NOT(ISERROR(SEARCH("-",C3)))</xm:f>
             <xm:f>"-"</xm:f>
             <x14:dxf>
@@ -1285,7 +1339,21 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C3:C15</xm:sqref>
+          <xm:sqref>C3:C12 C14:C16</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{E72C4E7F-760D-47EB-9372-BEA44B344FC9}">
+            <xm:f>NOT(ISERROR(SEARCH("-",C13)))</xm:f>
+            <xm:f>"-"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C13</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1328,7 +1396,7 @@
       <c r="C3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="25" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1339,14 +1407,14 @@
       <c r="C4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="26"/>
+      <c r="D4" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>6</v>
@@ -1379,7 +1447,7 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E8" s="17"/>
     </row>
@@ -1489,7 +1557,7 @@
       </c>
       <c r="C21" s="15"/>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
@@ -1498,7 +1566,7 @@
       </c>
       <c r="C22" s="15"/>
       <c r="D22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -1523,7 +1591,7 @@
       </c>
       <c r="C25" s="15"/>
       <c r="D25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -1532,7 +1600,7 @@
       </c>
       <c r="C26" s="15"/>
       <c r="D26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
@@ -1557,7 +1625,7 @@
       </c>
       <c r="C29" s="15"/>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
@@ -1590,7 +1658,7 @@
       </c>
       <c r="C33" s="15"/>
       <c r="D33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
@@ -1623,7 +1691,7 @@
       </c>
       <c r="C37" s="16"/>
       <c r="D37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1664,10 +1732,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0EDB92-DEAA-412F-9746-22ECF9A3453C}">
-  <dimension ref="B2:E24"/>
+  <dimension ref="B2:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1696,27 +1764,27 @@
       <c r="C3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="28" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="30"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
@@ -1738,7 +1806,7 @@
     </row>
     <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>6</v>
@@ -1747,7 +1815,7 @@
     </row>
     <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>10</v>
@@ -1756,7 +1824,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>6</v>
@@ -1765,11 +1833,11 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E11" s="17"/>
     </row>
@@ -1791,7 +1859,7 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="C14" s="15"/>
       <c r="E14" s="5"/>
@@ -1823,9 +1891,14 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="15"/>
+        <v>59</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>88</v>
+      </c>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -1837,46 +1910,37 @@
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="19" t="s">
+      <c r="C21" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="3"/>
+      <c r="C23" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E3:E5"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C23">
+  <conditionalFormatting sqref="C3:C22">
     <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
@@ -1901,7 +1965,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C3:C23</xm:sqref>
+          <xm:sqref>C3:C22</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1937,16 +2001,16 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="24"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E4" s="25"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E5" s="25"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="26"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>
@@ -1987,16 +2051,16 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="24"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E4" s="25"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E5" s="25"/>
+      <c r="E5" s="26"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="26"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>

</xml_diff>

<commit_message>
CommsTC Assign & Shutdown (Global & Kick)
</commit_message>
<xml_diff>
--- a/Development.xlsx
+++ b/Development.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\ISEC\SO2\Pratica\Trabalho\SOTaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BE1C0B-D469-4862-B3AA-93148D2DF692}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9164F42-D2B5-4063-9479-9CB678C16566}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="2280" windowWidth="21510" windowHeight="11430" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
+    <workbookView xWindow="5400" yWindow="945" windowWidth="21510" windowHeight="11430" activeTab="2" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
   </bookViews>
   <sheets>
     <sheet name="CenDLL" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="88">
   <si>
     <t>Functionality</t>
   </si>
@@ -1003,7 +1003,7 @@
   </sheetPr>
   <dimension ref="B2:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1159,7 +1159,7 @@
   </sheetPr>
   <dimension ref="B2:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1366,7 +1366,7 @@
   <dimension ref="B2:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1502,7 +1502,12 @@
       <c r="B15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>87</v>
+      </c>
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
@@ -1735,8 +1740,8 @@
   </sheetPr>
   <dimension ref="B2:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Taxi Kick - Doesn't allow kick while carrying passenger
</commit_message>
<xml_diff>
--- a/Development.xlsx
+++ b/Development.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\ISEC\SO2\Pratica\Trabalho\SOTaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4D27E4-F5D3-44EB-80C0-C5CBA6881338}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D91249-C8B9-4AE4-92A0-24FE3F009846}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="945" windowWidth="21510" windowHeight="11430" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
+    <workbookView xWindow="5745" yWindow="1290" windowWidth="21510" windowHeight="11430" activeTab="2" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
   </bookViews>
   <sheets>
     <sheet name="CenDLL" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="90">
   <si>
     <t>Functionality</t>
   </si>
@@ -274,9 +274,6 @@
   </si>
   <si>
     <t>ConPass</t>
-  </si>
-  <si>
-    <t>NamedPipe</t>
   </si>
   <si>
     <t>Receive notification (from central) to leave</t>
@@ -1012,7 +1009,7 @@
   </sheetPr>
   <dimension ref="B2:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -1066,7 +1063,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>6</v>
@@ -1126,7 +1123,7 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>6</v>
@@ -1177,7 +1174,7 @@
   <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,7 +1227,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>6</v>
@@ -1263,13 +1260,13 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>6</v>
@@ -1300,13 +1297,19 @@
       <c r="C13" s="15" t="s">
         <v>6</v>
       </c>
+      <c r="D13" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -1323,9 +1326,6 @@
       </c>
       <c r="C16" s="16" t="s">
         <v>6</v>
-      </c>
-      <c r="D16" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1394,8 +1394,8 @@
   </sheetPr>
   <dimension ref="B2:E38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,7 +1437,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="31"/>
     </row>
@@ -1452,13 +1452,13 @@
     </row>
     <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E6" s="17"/>
     </row>
@@ -1546,9 +1546,6 @@
       <c r="C16" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D16" t="s">
-        <v>87</v>
-      </c>
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -1635,9 +1632,6 @@
       <c r="C26" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D26" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
@@ -1645,7 +1639,7 @@
       </c>
       <c r="C27" s="15"/>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
@@ -1884,7 +1878,7 @@
       </c>
       <c r="C11" s="15"/>
       <c r="D11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E11" s="17"/>
     </row>
@@ -1906,7 +1900,7 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" s="15"/>
       <c r="E14" s="5"/>
@@ -1944,7 +1938,7 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E18" s="5"/>
     </row>

</xml_diff>

<commit_message>
Devolpment Update | TaxiDLL Communication -> Threads
</commit_message>
<xml_diff>
--- a/Development.xlsx
+++ b/Development.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\ISEC\SO2\Pratica\Trabalho\SOTaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BB7ED5-1FBC-4E1F-A1C5-6CF4A0EF55D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B737FA6F-CC6F-4FD2-BEB3-9A8260296182}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
+    <workbookView xWindow="4875" yWindow="2955" windowWidth="21510" windowHeight="11430" activeTab="4" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
   </bookViews>
   <sheets>
     <sheet name="CenDLL" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="98">
   <si>
     <t>Functionality</t>
   </si>
@@ -310,6 +310,31 @@
   </si>
   <si>
     <t>Close Named Pipe</t>
+  </si>
+  <si>
+    <t>It's an application developed to be used by a  manager of passengers, which means that only one instance will be running, while controlling several passengers.
+Passengers will ask for transports through this application.</t>
+  </si>
+  <si>
+    <t>Login Passengers</t>
+  </si>
+  <si>
+    <t>Receive Taxi Assignment to Passenger</t>
+  </si>
+  <si>
+    <t>Remove Passenger when arrive at destiny</t>
+  </si>
+  <si>
+    <t>Assumptions</t>
+  </si>
+  <si>
+    <t>- Passengers are not removed</t>
+  </si>
+  <si>
+    <t>List Passengers (from central?)</t>
+  </si>
+  <si>
+    <t>Connect named pipe to central</t>
   </si>
 </sst>
 </file>
@@ -493,7 +518,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1">
       <alignment horizontal="center" vertical="center"/>
@@ -577,13 +602,40 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableHeader" xfId="1" xr:uid="{14BB81CB-250E-410C-BBDF-11D0D22B1B10}"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="18">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1134,10 +1186,10 @@
     <mergeCell ref="E3:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C13">
-    <cfRule type="containsBlanks" dxfId="14" priority="1">
+    <cfRule type="containsBlanks" dxfId="17" priority="1">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="16" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1333,18 +1385,18 @@
     <mergeCell ref="E3:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C12 C14:C16">
-    <cfRule type="containsBlanks" dxfId="11" priority="4">
+    <cfRule type="containsBlanks" dxfId="14" priority="4">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="13" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="containsBlanks" dxfId="9" priority="1">
+    <cfRule type="containsBlanks" dxfId="12" priority="1">
       <formula>LEN(TRIM(C13))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C13)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1394,8 +1446,8 @@
   </sheetPr>
   <dimension ref="B2:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1527,7 +1579,9 @@
       <c r="B14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="15"/>
+      <c r="C14" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -1561,7 +1615,9 @@
       <c r="B18" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="15"/>
+      <c r="C18" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -1736,10 +1792,10 @@
     <mergeCell ref="E3:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C38">
-    <cfRule type="containsBlanks" dxfId="5" priority="1">
+    <cfRule type="containsBlanks" dxfId="8" priority="1">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1776,7 +1832,7 @@
   <dimension ref="B2:E23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1982,10 +2038,10 @@
     <mergeCell ref="E3:E5"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C22">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2016,10 +2072,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEB1183E-0A04-4BC9-83F9-3C193D2F4E32}">
-  <dimension ref="B2:E7"/>
+  <dimension ref="B2:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2042,26 +2098,116 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="29"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E4" s="30"/>
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="E3" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E5" s="30"/>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="31"/>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E7" s="2"/>
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="E7" s="27"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="E8" s="28"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="15"/>
+    </row>
+    <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="E10" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="27"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="27"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="27"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E3:E6"/>
+  <mergeCells count="2">
+    <mergeCell ref="E3:E8"/>
+    <mergeCell ref="E11:E15"/>
   </mergeCells>
+  <conditionalFormatting sqref="C3:C10">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
+      <formula>LEN(TRIM(C3))=0</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{BEDF2C12-0FC2-4905-A870-77E2AAA1DF79}">
+            <xm:f>NOT(ISERROR(SEARCH("-",C3)))</xm:f>
+            <xm:f>"-"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C3:C10</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Development Update | ConPass Arrival & Assignment Messages
</commit_message>
<xml_diff>
--- a/Development.xlsx
+++ b/Development.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\ISEC\SO2\Pratica\Trabalho\SOTaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CF12E3-731D-4F3D-A2A4-209F6884DB3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA27388-2480-4094-971A-F99677AAE4F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
   </bookViews>
   <sheets>
     <sheet name="CenDLL" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="99">
   <si>
     <t>Functionality</t>
   </si>
@@ -273,13 +273,7 @@
     <t>Clean String</t>
   </si>
   <si>
-    <t>ConPass</t>
-  </si>
-  <si>
     <t>Receive notification (from central) to leave</t>
-  </si>
-  <si>
-    <t>Named Pipe</t>
   </si>
   <si>
     <t>Missing MapInfo</t>
@@ -325,9 +319,6 @@
     <t>Assumptions</t>
   </si>
   <si>
-    <t>- Passengers are not removed</t>
-  </si>
-  <si>
     <t>Connect named pipe to central</t>
   </si>
   <si>
@@ -340,10 +331,13 @@
     <t>Receive Taxi Assigned to Passenger</t>
   </si>
   <si>
-    <t>Missing recover</t>
-  </si>
-  <si>
     <t>List Passengers</t>
+  </si>
+  <si>
+    <t>After movement is implemented</t>
+  </si>
+  <si>
+    <t>- Passengers are not removed by own choice</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +1118,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>6</v>
@@ -1184,7 +1178,7 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>6</v>
@@ -1235,7 +1229,7 @@
   <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,7 +1282,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>6</v>
@@ -1320,14 +1314,11 @@
       <c r="C9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D9" t="s">
-        <v>88</v>
-      </c>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>6</v>
@@ -1359,18 +1350,18 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -1455,8 +1446,8 @@
   </sheetPr>
   <dimension ref="B2:E38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1498,7 +1489,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E4" s="32"/>
     </row>
@@ -1513,13 +1504,10 @@
     </row>
     <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>86</v>
       </c>
       <c r="E6" s="17"/>
     </row>
@@ -1660,9 +1648,8 @@
       <c r="B22" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" t="s">
-        <v>77</v>
+      <c r="C22" s="15" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -1671,7 +1658,7 @@
       </c>
       <c r="C23" s="15"/>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -1702,9 +1689,8 @@
       <c r="B27" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" t="s">
-        <v>77</v>
+      <c r="C27" s="15" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
@@ -1727,9 +1713,8 @@
       <c r="B30" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="15"/>
-      <c r="D30" t="s">
-        <v>77</v>
+      <c r="C30" s="15" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
@@ -1941,9 +1926,8 @@
       <c r="B11" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" t="s">
-        <v>79</v>
+      <c r="C11" s="15" t="s">
+        <v>6</v>
       </c>
       <c r="E11" s="17"/>
     </row>
@@ -1965,7 +1949,7 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C14" s="15"/>
       <c r="E14" s="5"/>
@@ -2003,7 +1987,7 @@
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E18" s="5"/>
     </row>
@@ -2083,8 +2067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEB1183E-0A04-4BC9-83F9-3C193D2F4E32}">
   <dimension ref="B2:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2115,12 +2099,12 @@
         <v>6</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>6</v>
@@ -2129,7 +2113,7 @@
     </row>
     <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="26" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>6</v>
@@ -2138,7 +2122,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>6</v>
@@ -2147,27 +2131,29 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C7" s="15"/>
+        <v>95</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="E7" s="28"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C8" s="15"/>
+      <c r="D8" t="s">
+        <v>97</v>
+      </c>
       <c r="E8" s="29"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2178,7 +2164,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -2189,14 +2175,16 @@
         <v>6</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12" s="15"/>
+        <v>96</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="E12" s="28"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Path Introduction | x & y -> XY
</commit_message>
<xml_diff>
--- a/Development.xlsx
+++ b/Development.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\ISEC\SO2\Pratica\Trabalho\SOTaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA27388-2480-4094-971A-F99677AAE4F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3672484-74F9-48FC-8FBA-E10214239021}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="100">
   <si>
     <t>Functionality</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>- Passengers are not removed by own choice</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1708,6 +1711,9 @@
       <c r="C29" s="15" t="s">
         <v>6</v>
       </c>
+      <c r="E29" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">

</xml_diff>

<commit_message>
Remove Pass when Arrive | Taxi Random movement FIX
</commit_message>
<xml_diff>
--- a/Development.xlsx
+++ b/Development.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\ISEC\SO2\Pratica\Trabalho\SOTaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC66419-2062-4A81-A7B0-B2EED40C344F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0351B3EA-9C19-4B56-81A9-9610A72F98E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5445" yWindow="2205" windowWidth="21510" windowHeight="11430" activeTab="5" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
+    <workbookView xWindow="5490" yWindow="2280" windowWidth="21510" windowHeight="11430" activeTab="5" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
   </bookViews>
   <sheets>
     <sheet name="CenDLL" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="112">
   <si>
     <t>Functionality</t>
   </si>
@@ -2295,7 +2295,7 @@
   <dimension ref="B2:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,7 +2339,9 @@
       <c r="B5" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="14"/>
+      <c r="C5" s="14" t="s">
+        <v>6</v>
+      </c>
       <c r="E5" s="31"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -2385,7 +2387,9 @@
       <c r="B11" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="14"/>
+      <c r="C11" s="14" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="22" t="s">

</xml_diff>

<commit_message>
SOTaxi Final Adjustments S1
</commit_message>
<xml_diff>
--- a/Development.xlsx
+++ b/Development.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\ISEC\SO2\Pratica\Trabalho\SOTaxi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0351B3EA-9C19-4B56-81A9-9610A72F98E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7C0DA3-EC1C-4B84-8328-88F13E3D0DA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5490" yWindow="2280" windowWidth="21510" windowHeight="11430" activeTab="5" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{E3050521-E288-454E-983F-38C962347EC5}"/>
   </bookViews>
   <sheets>
     <sheet name="CenDLL" sheetId="4" r:id="rId1"/>
-    <sheet name="CTDLL" sheetId="2" r:id="rId2"/>
-    <sheet name="CenTaxi" sheetId="1" r:id="rId3"/>
+    <sheet name="CenTaxi" sheetId="1" r:id="rId2"/>
+    <sheet name="CTDLL" sheetId="2" r:id="rId3"/>
     <sheet name="ConTaxi" sheetId="5" r:id="rId4"/>
     <sheet name="ConPass" sheetId="3" r:id="rId5"/>
     <sheet name="MapInfo" sheetId="6" r:id="rId6"/>
@@ -37,8 +37,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ricardo Pereira</author>
+  </authors>
+  <commentList>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{A02EBF35-498D-45D2-8504-69D3B7A3973D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ricardo Pereira:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The size of the map adjusts to the size of the window… Always keeping a square form</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="122">
   <si>
     <t>Functionality</t>
   </si>
@@ -140,9 +174,6 @@
     <t>Share map to taxis and MapInfo</t>
   </si>
   <si>
-    <t>List taxis</t>
-  </si>
-  <si>
     <t>Set timeout for taxi&lt;-&gt;passenger assignment</t>
   </si>
   <si>
@@ -189,9 +220,6 @@
     <t>Default movement speed</t>
   </si>
   <si>
-    <t>Random movement (overwritten by autonomous)</t>
-  </si>
-  <si>
     <t>Send new position (when enter new cell)</t>
   </si>
   <si>
@@ -276,31 +304,19 @@
     <t>Receive notification (from central) to leave</t>
   </si>
   <si>
-    <t>Missing MapInfo</t>
-  </si>
-  <si>
     <t>Receive map</t>
   </si>
   <si>
     <t>Send new state</t>
   </si>
   <si>
-    <t>Missing Step</t>
-  </si>
-  <si>
     <t>Autonomous interest if between CDN</t>
   </si>
   <si>
     <t>Link to ImplicitDLL (Prof DLL)</t>
   </si>
   <si>
-    <t>Needs to be looked at</t>
-  </si>
-  <si>
     <t>Close handles</t>
-  </si>
-  <si>
-    <t>Needs completion</t>
   </si>
   <si>
     <t>Close Named Pipe</t>
@@ -322,9 +338,6 @@
     <t>Connect named pipe to central</t>
   </si>
   <si>
-    <t>Threads ready to lose connection and recover</t>
-  </si>
-  <si>
     <t>Ignore passengers when maxed out</t>
   </si>
   <si>
@@ -334,9 +347,6 @@
     <t>List Passengers</t>
   </si>
   <si>
-    <t>After movement is implemented</t>
-  </si>
-  <si>
     <t>- Passengers are not removed by own choice</t>
   </si>
   <si>
@@ -346,9 +356,6 @@
     <t>Get Map</t>
   </si>
   <si>
-    <t>Retry connection to central</t>
-  </si>
-  <si>
     <t>Structure</t>
   </si>
   <si>
@@ -358,12 +365,6 @@
     <t>Passengers</t>
   </si>
   <si>
-    <t>List</t>
-  </si>
-  <si>
-    <t>Transportations</t>
-  </si>
-  <si>
     <t>Setup Application</t>
   </si>
   <si>
@@ -377,13 +378,90 @@
   </si>
   <si>
     <t>Coordinates</t>
+  </si>
+  <si>
+    <t>It's a Win32 GUI Application to be used by anyone.
+This application displays the map, the taxis and passengers… Always updated and correct, allowing the user to control other application knowing what is happening or simply looking.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Transportations </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>*Transportations - Doesn't display bitmap but displays diferent text:</t>
+  </si>
+  <si>
+    <t>n - Taxi map identifier</t>
+  </si>
+  <si>
+    <t>Tn - Taxi n is moving randomly around the map</t>
+  </si>
+  <si>
+    <t>Yn - Taxi n is moving towards the passenger</t>
+  </si>
+  <si>
+    <t>Bn - Taxi n is has the passenger and moving towards the passenger destination</t>
+  </si>
+  <si>
+    <t>Display bitmaps</t>
+  </si>
+  <si>
+    <t>Edit bitmaps with dialog box</t>
+  </si>
+  <si>
+    <t>Mouse over | click actions</t>
+  </si>
+  <si>
+    <t>Random movement</t>
+  </si>
+  <si>
+    <t>Close App</t>
+  </si>
+  <si>
+    <t>Threads ready to lose connection</t>
+  </si>
+  <si>
+    <t>Bridge for Prof DLL functionality</t>
+  </si>
+  <si>
+    <t>Fields validations</t>
+  </si>
+  <si>
+    <t>Generate randoms</t>
+  </si>
+  <si>
+    <t>Calculate estimated time</t>
+  </si>
+  <si>
+    <t>Get Map's Cell neighbors</t>
+  </si>
+  <si>
+    <t>Get Path from A to B</t>
+  </si>
+  <si>
+    <t>List taxis/passengers</t>
+  </si>
+  <si>
+    <t>Send estimated time until arrival</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,6 +484,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -617,12 +708,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -643,13 +728,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="TableHeader" xfId="1" xr:uid="{14BB81CB-250E-410C-BBDF-11D0D22B1B10}"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill>
@@ -797,6 +886,27 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -813,6 +923,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1115,10 +1229,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:F13"/>
+  <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E18" sqref="E18:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,46 +1255,46 @@
       </c>
     </row>
     <row r="3" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>70</v>
-      </c>
       <c r="C4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="26"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="27"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="28"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="29"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
-        <v>71</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>10</v>
@@ -1188,52 +1302,100 @@
       <c r="E7" s="16"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="22" t="s">
+      <c r="C10" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="22" t="s">
+      <c r="C11" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="24"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="24"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="22" t="s">
-        <v>76</v>
-      </c>
       <c r="C12" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="22" t="s">
-        <v>87</v>
+      <c r="B13" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="C13" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1241,11 +1403,11 @@
   <mergeCells count="1">
     <mergeCell ref="E3:E6"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C13">
-    <cfRule type="containsBlanks" dxfId="20" priority="1">
+  <conditionalFormatting sqref="C3:C19">
+    <cfRule type="containsBlanks" dxfId="23" priority="1">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1266,7 +1428,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C3:C13</xm:sqref>
+          <xm:sqref>C3:C19</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1275,6 +1437,387 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829518F3-E732-4739-88CC-0EF1DA64B468}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B2:E38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="48" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="30"/>
+    </row>
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="16"/>
+    </row>
+    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="16"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="16"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="16"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="16"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E3:E4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C3:C38">
+    <cfRule type="containsBlanks" dxfId="20" priority="1">
+      <formula>LEN(TRIM(C3))=0</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="66" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{DC704FD4-8FB9-49D6-AC04-C437999A6A74}">
+            <xm:f>NOT(ISERROR(SEARCH("-",C3)))</xm:f>
+            <xm:f>"-"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C3:C38</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{958854CD-AF03-4FB5-B1A5-A2453B181DC1}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -1282,7 +1825,7 @@
   <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,40 +1854,40 @@
       <c r="C3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="29"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="32"/>
+      <c r="E6" s="30"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>10</v>
@@ -1353,7 +1896,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>6</v>
@@ -1362,7 +1905,7 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>6</v>
@@ -1371,7 +1914,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>6</v>
@@ -1380,7 +1923,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>6</v>
@@ -1389,7 +1932,7 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>10</v>
@@ -1397,24 +1940,18 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -1427,7 +1964,7 @@
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="19" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>6</v>
@@ -1492,397 +2029,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829518F3-E732-4739-88CC-0EF1DA64B468}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="B2:E38"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="48" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="32"/>
-    </row>
-    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="16"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="16"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="16"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="16"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="14"/>
-      <c r="D23" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E3:E4"/>
-  </mergeCells>
-  <conditionalFormatting sqref="C3:C38">
-    <cfRule type="containsBlanks" dxfId="11" priority="1">
-      <formula>LEN(TRIM(C3))=0</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",C3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="66" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{DC704FD4-8FB9-49D6-AC04-C437999A6A74}">
-            <xm:f>NOT(ISERROR(SEARCH("-",C3)))</xm:f>
-            <xm:f>"-"</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="7" tint="0.59996337778862885"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C3:C38</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C0EDB92-DEAA-412F-9746-22ECF9A3453C}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:E23"/>
+  <dimension ref="B2:E24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C21"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,32 +2061,32 @@
     </row>
     <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="27" t="s">
-        <v>43</v>
+      <c r="E3" s="25" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
@@ -1944,7 +2099,7 @@
     </row>
     <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>6</v>
@@ -1953,7 +2108,7 @@
     </row>
     <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>6</v>
@@ -1962,7 +2117,7 @@
     </row>
     <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>10</v>
@@ -1971,7 +2126,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>6</v>
@@ -1980,7 +2135,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>6</v>
@@ -1998,99 +2153,111 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="14"/>
+        <v>45</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>6</v>
+      </c>
       <c r="E13" s="16"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="E14" s="4"/>
+        <v>121</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="16"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C17" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="14"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="18" t="s">
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="2"/>
+      <c r="C23" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E3:E5"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C22">
-    <cfRule type="containsBlanks" dxfId="8" priority="1">
+  <conditionalFormatting sqref="C3:C23">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2111,7 +2278,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C3:C22</xm:sqref>
+          <xm:sqref>C3:C23</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2124,7 +2291,7 @@
   <dimension ref="B2:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2154,103 +2321,108 @@
       <c r="C3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="26"/>
+    </row>
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="26"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="26"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="24" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="28"/>
-    </row>
-    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="28"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="28"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>95</v>
-      </c>
       <c r="C7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="28"/>
+      <c r="E7" s="26"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" t="s">
-        <v>97</v>
-      </c>
-      <c r="E8" s="29"/>
+      <c r="B8" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="27"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>93</v>
+      <c r="B9" s="24" t="s">
+        <v>113</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="33" t="s">
-        <v>98</v>
+      <c r="E11" s="31" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="22" t="s">
-        <v>96</v>
+      <c r="B12" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="26"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E13" s="28"/>
+      <c r="B13" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="26"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E14" s="28"/>
+      <c r="E14" s="26"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E15" s="29"/>
+      <c r="E15" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2258,11 +2430,19 @@
     <mergeCell ref="E3:E8"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:C12">
-    <cfRule type="containsBlanks" dxfId="5" priority="1">
+    <cfRule type="containsBlanks" dxfId="11" priority="4">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="containsBlanks" dxfId="8" priority="1">
+      <formula>LEN(TRIM(C13))=0</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",C13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2271,7 +2451,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{BEDF2C12-0FC2-4905-A870-77E2AAA1DF79}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{BEDF2C12-0FC2-4905-A870-77E2AAA1DF79}">
             <xm:f>NOT(ISERROR(SEARCH("-",C3)))</xm:f>
             <xm:f>"-"</xm:f>
             <x14:dxf>
@@ -2284,6 +2464,20 @@
           </x14:cfRule>
           <xm:sqref>C3:C12</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{9A4294BB-4FDA-43AC-9F67-F1FBC1A70EE1}">
+            <xm:f>NOT(ISERROR(SEARCH("-",C13)))</xm:f>
+            <xm:f>"-"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>C13</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -2291,11 +2485,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{479F52BC-D323-484C-B995-079999EECDCA}">
-  <dimension ref="B2:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{479F52BC-D323-484C-B995-079999EECDCA}">
+  <dimension ref="B2:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:C7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2318,130 +2512,160 @@
       </c>
     </row>
     <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="26"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="26"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="26"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="E7" s="27"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="E8" s="16"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="E9" s="16"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="30"/>
-    </row>
-    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="31"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="31"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="31"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="E7" s="32"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="C12" s="14"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="C13" s="14"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="14"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="14"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E3:E7"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:C17">
-    <cfRule type="containsBlanks" dxfId="2" priority="1">
+  <conditionalFormatting sqref="C3:C16">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -2457,7 +2681,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C3:C17</xm:sqref>
+          <xm:sqref>C3:C16</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>